<commit_message>
Integrate SheetsJS for reading full spreadsheets (not just CSV files) directly. Repair corrupted sample-names.csv file.
</commit_message>
<xml_diff>
--- a/testing/data/sample-names.xlsx
+++ b/testing/data/sample-names.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Macintosh" sheetId="1" r:id="rId1"/>
-    <sheet name="Windows ANSI" sheetId="2" r:id="rId2"/>
-    <sheet name="DOS PC-8" sheetId="3" r:id="rId3"/>
-    <sheet name="Western DOS Latin-1" sheetId="4" r:id="rId4"/>
-    <sheet name="Western Mac Roman" sheetId="5" r:id="rId5"/>
+    <sheet name="Western Mac Roman" sheetId="5" r:id="rId1"/>
+    <sheet name="Macintosh" sheetId="1" r:id="rId2"/>
+    <sheet name="Windows ANSI" sheetId="2" r:id="rId3"/>
+    <sheet name="DOS PC-8" sheetId="3" r:id="rId4"/>
+    <sheet name="Western DOS Latin-1" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="sample_names" localSheetId="2">'DOS PC-8'!$A$1:$D$83</definedName>
-    <definedName name="sample_names" localSheetId="0">Macintosh!$A$1:$D$83</definedName>
-    <definedName name="sample_names" localSheetId="3">'Western DOS Latin-1'!$A$1:$D$83</definedName>
-    <definedName name="sample_names" localSheetId="4">'Western Mac Roman'!$A$1:$D$83</definedName>
-    <definedName name="sample_names" localSheetId="1">'Windows ANSI'!$A$1:$D$83</definedName>
+    <definedName name="sample_names" localSheetId="3">'DOS PC-8'!$A$1:$D$83</definedName>
+    <definedName name="sample_names" localSheetId="1">Macintosh!$A$1:$D$83</definedName>
+    <definedName name="sample_names" localSheetId="4">'Western DOS Latin-1'!$A$1:$D$83</definedName>
+    <definedName name="sample_names" localSheetId="0">'Western Mac Roman'!$A$1:$D$83</definedName>
+    <definedName name="sample_names" localSheetId="2">'Windows ANSI'!$A$1:$D$83</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -72,7 +72,7 @@
     </textPr>
   </connection>
   <connection id="5" name="sample-names.csv4" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="MBP17:Users:jeffpiazza:Cub Scouts:Pinewood Derby:Software Development:derbynet:testing:data:sample-names.csv" comma="1">
+    <textPr sourceFile="MBP17:Users:jeffpiazza:Cub Scouts:Pinewood Derby:Software Development:derbynet:testing:data:sample-names.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -654,23 +654,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sample-names" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sample-names" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sample-names" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sample-names" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sample-names" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sample-names" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -997,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="400" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1057,7 +1057,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D4">
         <v>103</v>
@@ -1127,7 +1127,7 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D9">
         <v>108</v>
@@ -1197,7 +1197,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D14">
         <v>113</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>173</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
@@ -1267,7 +1267,7 @@
         <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D19">
         <v>118</v>
@@ -1337,7 +1337,7 @@
         <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D24">
         <v>123</v>
@@ -1407,7 +1407,7 @@
         <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D29">
         <v>128</v>
@@ -1477,7 +1477,7 @@
         <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D34">
         <v>133</v>
@@ -1547,7 +1547,7 @@
         <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D39">
         <v>138</v>
@@ -1617,7 +1617,7 @@
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D44">
         <v>143</v>
@@ -1687,7 +1687,7 @@
         <v>102</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D49">
         <v>148</v>
@@ -1757,7 +1757,7 @@
         <v>112</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D54">
         <v>153</v>
@@ -1827,7 +1827,7 @@
         <v>122</v>
       </c>
       <c r="C59" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D59">
         <v>158</v>
@@ -1897,7 +1897,7 @@
         <v>132</v>
       </c>
       <c r="C64" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D64">
         <v>163</v>
@@ -1967,7 +1967,7 @@
         <v>142</v>
       </c>
       <c r="C69" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D69">
         <v>168</v>
@@ -2037,7 +2037,7 @@
         <v>152</v>
       </c>
       <c r="C74" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D74">
         <v>173</v>
@@ -2107,7 +2107,7 @@
         <v>162</v>
       </c>
       <c r="C79" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="D79">
         <v>178</v>
@@ -3429,7 +3429,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>103</v>
@@ -3499,7 +3499,7 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <v>108</v>
@@ -3569,7 +3569,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <v>113</v>
@@ -3591,7 +3591,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
@@ -3639,7 +3639,7 @@
         <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D19">
         <v>118</v>
@@ -3709,7 +3709,7 @@
         <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D24">
         <v>123</v>
@@ -3779,7 +3779,7 @@
         <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D29">
         <v>128</v>
@@ -3849,7 +3849,7 @@
         <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D34">
         <v>133</v>
@@ -3919,7 +3919,7 @@
         <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D39">
         <v>138</v>
@@ -3989,7 +3989,7 @@
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D44">
         <v>143</v>
@@ -4059,7 +4059,7 @@
         <v>102</v>
       </c>
       <c r="C49" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D49">
         <v>148</v>
@@ -4129,7 +4129,7 @@
         <v>112</v>
       </c>
       <c r="C54" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D54">
         <v>153</v>
@@ -4199,7 +4199,7 @@
         <v>122</v>
       </c>
       <c r="C59" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D59">
         <v>158</v>
@@ -4269,7 +4269,7 @@
         <v>132</v>
       </c>
       <c r="C64" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D64">
         <v>163</v>
@@ -4339,7 +4339,7 @@
         <v>142</v>
       </c>
       <c r="C69" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D69">
         <v>168</v>
@@ -4409,7 +4409,7 @@
         <v>152</v>
       </c>
       <c r="C74" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D74">
         <v>173</v>
@@ -4479,7 +4479,7 @@
         <v>162</v>
       </c>
       <c r="C79" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="D79">
         <v>178</v>
@@ -4552,6 +4552,1192 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D83"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" t="s">
+        <v>170</v>
+      </c>
+      <c r="D34">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" t="s">
+        <v>170</v>
+      </c>
+      <c r="D49">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>107</v>
+      </c>
+      <c r="B52" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" t="s">
+        <v>170</v>
+      </c>
+      <c r="D59">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>129</v>
+      </c>
+      <c r="B63" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" t="s">
+        <v>170</v>
+      </c>
+      <c r="D64">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>133</v>
+      </c>
+      <c r="B65" t="s">
+        <v>134</v>
+      </c>
+      <c r="C65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>135</v>
+      </c>
+      <c r="B66" t="s">
+        <v>136</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>137</v>
+      </c>
+      <c r="B67" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68" t="s">
+        <v>140</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>141</v>
+      </c>
+      <c r="B69" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" t="s">
+        <v>170</v>
+      </c>
+      <c r="D69">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>143</v>
+      </c>
+      <c r="B70" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>145</v>
+      </c>
+      <c r="B71" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>147</v>
+      </c>
+      <c r="B72" t="s">
+        <v>148</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>149</v>
+      </c>
+      <c r="B73" t="s">
+        <v>150</v>
+      </c>
+      <c r="C73" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" t="s">
+        <v>170</v>
+      </c>
+      <c r="D74">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>153</v>
+      </c>
+      <c r="B75" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>155</v>
+      </c>
+      <c r="B76" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>157</v>
+      </c>
+      <c r="B77" t="s">
+        <v>158</v>
+      </c>
+      <c r="C77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>159</v>
+      </c>
+      <c r="B78" t="s">
+        <v>160</v>
+      </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>161</v>
+      </c>
+      <c r="B79" t="s">
+        <v>162</v>
+      </c>
+      <c r="C79" t="s">
+        <v>170</v>
+      </c>
+      <c r="D79">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>163</v>
+      </c>
+      <c r="B80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C80" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" t="s">
+        <v>166</v>
+      </c>
+      <c r="C81" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" t="s">
+        <v>169</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
@@ -5737,1190 +6923,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D83"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="400" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D9">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>172</v>
-      </c>
-      <c r="D14">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>173</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" t="s">
-        <v>172</v>
-      </c>
-      <c r="D19">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" t="s">
-        <v>172</v>
-      </c>
-      <c r="D24">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>172</v>
-      </c>
-      <c r="D29">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" t="s">
-        <v>172</v>
-      </c>
-      <c r="D34">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>76</v>
-      </c>
-      <c r="B36" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" t="s">
-        <v>172</v>
-      </c>
-      <c r="D39">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>86</v>
-      </c>
-      <c r="B41" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" t="s">
-        <v>172</v>
-      </c>
-      <c r="D44">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>94</v>
-      </c>
-      <c r="B45" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
-        <v>98</v>
-      </c>
-      <c r="B47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" t="s">
-        <v>102</v>
-      </c>
-      <c r="C49" t="s">
-        <v>172</v>
-      </c>
-      <c r="D49">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
-        <v>103</v>
-      </c>
-      <c r="B50" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
-        <v>105</v>
-      </c>
-      <c r="B51" t="s">
-        <v>106</v>
-      </c>
-      <c r="C51" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
-        <v>107</v>
-      </c>
-      <c r="B52" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" t="s">
-        <v>109</v>
-      </c>
-      <c r="B53" t="s">
-        <v>110</v>
-      </c>
-      <c r="C53" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
-        <v>111</v>
-      </c>
-      <c r="B54" t="s">
-        <v>112</v>
-      </c>
-      <c r="C54" t="s">
-        <v>172</v>
-      </c>
-      <c r="D54">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
-        <v>113</v>
-      </c>
-      <c r="B55" t="s">
-        <v>114</v>
-      </c>
-      <c r="C55" t="s">
-        <v>15</v>
-      </c>
-      <c r="D55">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B56" t="s">
-        <v>116</v>
-      </c>
-      <c r="C56" t="s">
-        <v>18</v>
-      </c>
-      <c r="D56">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
-        <v>117</v>
-      </c>
-      <c r="B57" t="s">
-        <v>118</v>
-      </c>
-      <c r="C57" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>121</v>
-      </c>
-      <c r="B59" t="s">
-        <v>122</v>
-      </c>
-      <c r="C59" t="s">
-        <v>172</v>
-      </c>
-      <c r="D59">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
-        <v>123</v>
-      </c>
-      <c r="B60" t="s">
-        <v>124</v>
-      </c>
-      <c r="C60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>125</v>
-      </c>
-      <c r="B61" t="s">
-        <v>126</v>
-      </c>
-      <c r="C61" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
-        <v>127</v>
-      </c>
-      <c r="B62" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
-        <v>129</v>
-      </c>
-      <c r="B63" t="s">
-        <v>130</v>
-      </c>
-      <c r="C63" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
-        <v>131</v>
-      </c>
-      <c r="B64" t="s">
-        <v>132</v>
-      </c>
-      <c r="C64" t="s">
-        <v>172</v>
-      </c>
-      <c r="D64">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" t="s">
-        <v>133</v>
-      </c>
-      <c r="B65" t="s">
-        <v>134</v>
-      </c>
-      <c r="C65" t="s">
-        <v>15</v>
-      </c>
-      <c r="D65">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
-        <v>135</v>
-      </c>
-      <c r="B66" t="s">
-        <v>136</v>
-      </c>
-      <c r="C66" t="s">
-        <v>18</v>
-      </c>
-      <c r="D66">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" t="s">
-        <v>137</v>
-      </c>
-      <c r="B67" t="s">
-        <v>138</v>
-      </c>
-      <c r="C67" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" t="s">
-        <v>139</v>
-      </c>
-      <c r="B68" t="s">
-        <v>140</v>
-      </c>
-      <c r="C68" t="s">
-        <v>9</v>
-      </c>
-      <c r="D68">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" t="s">
-        <v>141</v>
-      </c>
-      <c r="B69" t="s">
-        <v>142</v>
-      </c>
-      <c r="C69" t="s">
-        <v>172</v>
-      </c>
-      <c r="D69">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" t="s">
-        <v>143</v>
-      </c>
-      <c r="B70" t="s">
-        <v>144</v>
-      </c>
-      <c r="C70" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" t="s">
-        <v>145</v>
-      </c>
-      <c r="B71" t="s">
-        <v>146</v>
-      </c>
-      <c r="C71" t="s">
-        <v>18</v>
-      </c>
-      <c r="D71">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" t="s">
-        <v>147</v>
-      </c>
-      <c r="B72" t="s">
-        <v>148</v>
-      </c>
-      <c r="C72" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" t="s">
-        <v>149</v>
-      </c>
-      <c r="B73" t="s">
-        <v>150</v>
-      </c>
-      <c r="C73" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" t="s">
-        <v>151</v>
-      </c>
-      <c r="B74" t="s">
-        <v>152</v>
-      </c>
-      <c r="C74" t="s">
-        <v>172</v>
-      </c>
-      <c r="D74">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" t="s">
-        <v>153</v>
-      </c>
-      <c r="B75" t="s">
-        <v>154</v>
-      </c>
-      <c r="C75" t="s">
-        <v>15</v>
-      </c>
-      <c r="D75">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" t="s">
-        <v>155</v>
-      </c>
-      <c r="B76" t="s">
-        <v>156</v>
-      </c>
-      <c r="C76" t="s">
-        <v>18</v>
-      </c>
-      <c r="D76">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" t="s">
-        <v>157</v>
-      </c>
-      <c r="B77" t="s">
-        <v>158</v>
-      </c>
-      <c r="C77" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" t="s">
-        <v>159</v>
-      </c>
-      <c r="B78" t="s">
-        <v>160</v>
-      </c>
-      <c r="C78" t="s">
-        <v>9</v>
-      </c>
-      <c r="D78">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" t="s">
-        <v>161</v>
-      </c>
-      <c r="B79" t="s">
-        <v>162</v>
-      </c>
-      <c r="C79" t="s">
-        <v>172</v>
-      </c>
-      <c r="D79">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" t="s">
-        <v>163</v>
-      </c>
-      <c r="B80" t="s">
-        <v>164</v>
-      </c>
-      <c r="C80" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" t="s">
-        <v>165</v>
-      </c>
-      <c r="B81" t="s">
-        <v>166</v>
-      </c>
-      <c r="C81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D81">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" t="s">
-        <v>167</v>
-      </c>
-      <c r="B82" t="s">
-        <v>168</v>
-      </c>
-      <c r="C82" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" t="s">
-        <v>167</v>
-      </c>
-      <c r="B83" t="s">
-        <v>169</v>
-      </c>
-      <c r="C83" t="s">
-        <v>9</v>
-      </c>
-      <c r="D83">
-        <v>182</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>